<commit_message>
Require user to select folder full of scripts, display this on the frontend, wn
</commit_message>
<xml_diff>
--- a/local_helper/local_data/sample_data.xlsx
+++ b/local_helper/local_data/sample_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numbers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Numbers" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,21 @@
           <t>Column B</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Mean</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sum</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,6 +467,15 @@
       <c r="B2" t="n">
         <v>5</v>
       </c>
+      <c r="C2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -460,6 +484,15 @@
       <c r="B3" t="n">
         <v>15</v>
       </c>
+      <c r="C3" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>300</v>
+      </c>
+      <c r="E3" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -468,6 +501,15 @@
       <c r="B4" t="n">
         <v>25</v>
       </c>
+      <c r="C4" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>750</v>
+      </c>
+      <c r="E4" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -476,6 +518,15 @@
       <c r="B5" t="n">
         <v>35</v>
       </c>
+      <c r="C5" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="E5" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -483,6 +534,15 @@
       </c>
       <c r="B6" t="n">
         <v>45</v>
+      </c>
+      <c r="C6" t="n">
+        <v>47.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2250</v>
+      </c>
+      <c r="E6" t="n">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted Docker and unused files
</commit_message>
<xml_diff>
--- a/local_helper/local_data/sample_data.xlsx
+++ b/local_helper/local_data/sample_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Numbers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Numbers" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>